<commit_message>
update before next changes.
</commit_message>
<xml_diff>
--- a/etl_driver.xlsx
+++ b/etl_driver.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j/Documents/code/_public_github/python/python_excel_driven_etl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B8C8E6-D5B3-094D-82A4-E78F94F6694B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9692E2-86DE-3143-B18F-D0277C65AC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18320" yWindow="4680" windowWidth="13660" windowHeight="15680" xr2:uid="{DD8FF89A-F853-9A47-ABCA-B425F38C1F8B}"/>
+    <workbookView xWindow="19500" yWindow="920" windowWidth="13660" windowHeight="15680" xr2:uid="{DD8FF89A-F853-9A47-ABCA-B425F38C1F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Fitst completely working version.  Still more things to add.
</commit_message>
<xml_diff>
--- a/etl_driver.xlsx
+++ b/etl_driver.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j/Documents/code/_public_github/python/python_excel_driven_etl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9692E2-86DE-3143-B18F-D0277C65AC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB34DAA-C416-9444-9E0E-A337B37B95B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19500" yWindow="920" windowWidth="13660" windowHeight="15680" xr2:uid="{DD8FF89A-F853-9A47-ABCA-B425F38C1F8B}"/>
+    <workbookView xWindow="16640" yWindow="1960" windowWidth="13660" windowHeight="15680" activeTab="3" xr2:uid="{DD8FF89A-F853-9A47-ABCA-B425F38C1F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
-    <sheet name="orders" sheetId="3" r:id="rId2"/>
-    <sheet name="order_details" sheetId="4" r:id="rId3"/>
+    <sheet name="customers" sheetId="5" r:id="rId2"/>
+    <sheet name="orders" sheetId="3" r:id="rId3"/>
+    <sheet name="order_details" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>customer_id</t>
   </si>
@@ -124,6 +125,45 @@
   </si>
   <si>
     <t>nw_dest_pg</t>
+  </si>
+  <si>
+    <t>company_name</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>contact_title</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>postal_code</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Columns</t>
+  </si>
+  <si>
+    <t>xfax</t>
+  </si>
+  <si>
+    <t>xphone</t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>New_name</t>
   </si>
 </sst>
 </file>
@@ -487,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5C00C10-28E4-E747-8D69-27AACF1D15E8}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -553,11 +593,95 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7878B05C-5D27-734B-A074-7CC2C7CCBE43}">
-  <dimension ref="A1:A14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA5C86EF-0271-7D4C-B4B2-1AF01B8FDA7F}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7878B05C-5D27-734B-A074-7CC2C7CCBE43}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,73 +689,84 @@
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
@@ -640,12 +775,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0C3C7F-36D4-0049-981E-22A70AB1CF1C}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -653,28 +788,39 @@
     <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>